<commit_message>
added preliminary control vhdl
-updated the excel file
-added a first version of the preliminary control
</commit_message>
<xml_diff>
--- a/IO_list.xlsx
+++ b/IO_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politecnicobari-my.sharepoint.com/personal/f_stasi2_studenti_poliba_it/Documents/UNI_Digital_Programmable_Systems/VHDLProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\VHDLProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="8_{FAE11CC4-EDAA-4B09-96C6-1E093115AA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78A855DD-587F-4DB6-8F8A-FC33D0028546}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CEF562-17E9-4727-8EEA-24D3443ADF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7F93D5CB-CF8E-4947-B349-B01380E8BF50}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7F93D5CB-CF8E-4947-B349-B01380E8BF50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
   <si>
     <t>byte_divider</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>high value if there is a new data</t>
+  </si>
+  <si>
+    <t>CLK3</t>
   </si>
 </sst>
 </file>
@@ -246,18 +249,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Neutrale" xfId="1" builtinId="28"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -277,12 +281,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -598,29 +598,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29477555-0DE6-4222-AA4A-F1B072AFF671}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -634,7 +634,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -644,7 +644,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>46</v>
       </c>
@@ -656,7 +656,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>47</v>
       </c>
@@ -668,7 +668,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
@@ -680,15 +680,15 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -702,113 +702,111 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>15</v>
@@ -818,246 +816,258 @@
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="23" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="24" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D48" s="2"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D49" s="2"/>
+      <c r="D50" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A32:D32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>